<commit_message>
update with 16 points
</commit_message>
<xml_diff>
--- a/SEO-audit.xlsx
+++ b/SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cycki\Desktop\Openclassroom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DC0EEBE-5CE8-47A7-A150-AECD00AFD49F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0024CBD-381F-4D1C-B0A4-A5E4B81EF888}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>Category</t>
   </si>
@@ -60,9 +60,6 @@
     <t>https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links</t>
   </si>
   <si>
-    <t>hidden text in footer</t>
-  </si>
-  <si>
     <t>SEO</t>
   </si>
   <si>
@@ -94,70 +91,144 @@
   </si>
   <si>
     <t>lang attribute in &lt;html&gt; tag set to "default" instead of actual language</t>
+  </si>
+  <si>
+    <t>WCAG Success Criterion 3.1.1 requires that a page language is specified in a way which may be 'programmatically determined' (i.e. via the lang attribute).</t>
+  </si>
+  <si>
+    <t>External links in footer</t>
+  </si>
+  <si>
+    <t>Avoid placing external links in your footer. If you must link to another website in your footer, use the “nofollow” tag.</t>
+  </si>
+  <si>
+    <t>Links to external websites in the footer used to rank up in SEO are considered a "black hat" technique which might result in the website being banned from search engines results</t>
+  </si>
+  <si>
+    <t>Using text and visuals as one image is preventing assistive technology users to preceive the content as for example readers won't be able to select text. It is also preventing people from modifying fonts and doesn’t respond to changes in color, size, and regular text.</t>
+  </si>
+  <si>
+    <t>Separate the text and place it as HTML content on top of the background or communicate all of the text in the image as alternative text.</t>
+  </si>
+  <si>
+    <t>Irrelevant links to partners</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/en/courses/3594061-drive-traffic-to-your-website-with-search-engine-optimization-seo/5838332-increase-your-websites-authority</t>
+  </si>
+  <si>
+    <t>A quality link to/from your website should be found among content that is relevant to your profession.
+It should also attract real traffic, meaning that it is on a page real visitors read, not hidden away in some obscure part of the website.</t>
+  </si>
+  <si>
+    <t>Increase your website authority by using only quality links to/from other websites and building relevant partnerships.</t>
   </si>
   <si>
     <t>https://www.w3schools.com/tags/tag_title.asp
 https://openclassrooms.com/en/courses/3594061-drive-traffic-to-your-website-with-search-engine-optimization-seo/5838156-optimize-the-content-of-your-web-pages</t>
   </si>
   <si>
-    <r>
-      <t>WCAG Success Criterion 3.1.1 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF212121"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>requires</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF212121"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t> that a page language is specified in a way which may be 'programmatically determined' (i.e. via the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF212121"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>lang</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF212121"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t> attribute).</t>
-    </r>
-  </si>
-  <si>
-    <t>https://www.w3.org/WAI/tutorials/images/textual/</t>
-  </si>
-  <si>
-    <t>Text on images</t>
+    <t>https://www.w3.org/WAI/tutorials/images/textual/
+https://openclassrooms.com/en/courses/6663451-make-your-web-content-accessible/6912083-get-to-know-the-web-content-accessibility-guidelines-wcag</t>
+  </si>
+  <si>
+    <t>https://robpowellbizblog.com/seo-footer-best-practices
+https://openclassrooms.com/en/courses/3594061-drive-traffic-to-your-website-with-search-engine-optimization-seo/5838332-increase-your-websites-authority</t>
+  </si>
+  <si>
+    <t>Text on images/missing h2 tags in their place</t>
+  </si>
+  <si>
+    <t>Multiple &lt;h1&gt; tags on the website</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/en/courses/3594061-drive-traffic-to-your-website-with-search-engine-optimization-seo/5838156-optimize-the-content-of-your-web-pages</t>
+  </si>
+  <si>
+    <t>The keywords for the website should be included in titles, &lt;h1&gt; (as an exact match to title) and &lt;h2&gt; tags, paragraphs and alternative text in images where possible.</t>
+  </si>
+  <si>
+    <t>Missing keywords in &lt;h1&gt; tag, &lt;h2&gt; tags</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/en/courses/1306056-ensure-your-website-meets-technical-seo-requirements/6200762-keep-your-webpages-light</t>
+  </si>
+  <si>
+    <t>The larger the image, the bigger the file, and the longer it takes for a browser to download. Using not optimized images will slow loading your page for users.</t>
+  </si>
+  <si>
+    <t>Always keep your images as light in size as possible</t>
+  </si>
+  <si>
+    <t>Image file names missing or irrelevant to pictures content</t>
+  </si>
+  <si>
+    <t>https://www.searchenginejournal.com/on-page-seo/image-optimization/</t>
+  </si>
+  <si>
+    <t>Image file names alert Google and other search engine crawlers as to the subject matter of the image.</t>
+  </si>
+  <si>
+    <t>Change the file name from the default to help the search engines understand your image and improve your SEO value.</t>
+  </si>
+  <si>
+    <t>hidden text/keywords in footer and header</t>
+  </si>
+  <si>
+    <t>Move text from bloc-5 to the front</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/en/courses/6663451-make-your-web-content-accessible/6912083-get-to-know-the-web-content-accessibility-guidelines-wcag</t>
+  </si>
+  <si>
+    <t>Text should be placed as HTML content on top of the background not be hidden behind it.</t>
+  </si>
+  <si>
+    <t>Always make sure that text on your website is not hidden behind other elements and that it is possible to select it.</t>
+  </si>
+  <si>
+    <t>Images size is not optimized and incorrect format</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/en/courses/1306056-ensure-your-website-meets-technical-seo-requirements/6200762-keep-your-webpages-light
+https://developers.google.com/speed/webp</t>
+  </si>
+  <si>
+    <t>CSS and javaScript not minified</t>
+  </si>
+  <si>
+    <t>Minifying a file means removing unnecessary characters (spaces, line breaks, comments, block separators) from the file, which drastically reduces its file size. It increases the loading speed.</t>
+  </si>
+  <si>
+    <t>Always minify all .css and .js files to increase loading speed.</t>
+  </si>
+  <si>
+    <t>If you don't set the call to your JavaScript files correctly, they will prevent the page from being displayed before it's fully loaded.</t>
+  </si>
+  <si>
+    <t>javaScript loading at the same time as HTML</t>
+  </si>
+  <si>
+    <t>If the execution order is not important and the scripts can be executed as soon as they are available, use the asynchronous method.</t>
+  </si>
+  <si>
+    <t>a lot of unsused CSS in the website files</t>
+  </si>
+  <si>
+    <t>https://web.dev/unused-css-rules/?utm_source=lighthouse&amp;utm_medium=devtools</t>
+  </si>
+  <si>
+    <t>By default, a browser must download, parse, and process all external stylesheets that it encounters before it can display, or render, any content to a user's screen. It wouldn't make sense for a browser to attempt to display content before the stylesheets have been processed, because the stylesheets may contain rules that affect the styling of the page.</t>
+  </si>
+  <si>
+    <t>Remove the unused CSS to reduce unnecessary bytes consumed by network activity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -182,12 +253,61 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
@@ -195,30 +315,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF212121"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
+      <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF212121"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
+      <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,8 +340,28 @@
         <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -247,48 +376,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -501,268 +671,350 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
-    <col min="6" max="6" width="44.33203125" customWidth="1"/>
-    <col min="7" max="26" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.33203125" style="1" customWidth="1"/>
+    <col min="7" max="26" width="10.5546875" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="11.21875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
-    <row r="2" spans="1:26" ht="63" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:26" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="b">
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="63" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>21</v>
+    <row r="3" spans="1:26" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="b">
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="C7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" ht="63" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="8" spans="1:26" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4" t="b">
+      <c r="B8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>10</v>
+      <c r="F8" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="63" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="4" t="b">
+    <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>17</v>
+      <c r="F9" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="b">
+    <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>25</v>
+      <c r="F10" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="11" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="b">
+      <c r="B11" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F11" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="12" spans="1:26" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="b">
+      <c r="B12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F12" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="13" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4" t="b">
+      <c r="B13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F13" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="14" spans="1:26" ht="63" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="b">
+      <c r="B14" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F10" s="10"/>
+      <c r="F14" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="10"/>
+    <row r="15" spans="1:26" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="10"/>
+    <row r="16" spans="1:26" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1746,9 +1998,8 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
performance audit and minifying
</commit_message>
<xml_diff>
--- a/SEO-audit.xlsx
+++ b/SEO-audit.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cycki\Desktop\Openclassroom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cycki\Desktop\Openclassroom\project4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0024CBD-381F-4D1C-B0A4-A5E4B81EF888}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221F506B-291C-4595-B3BE-0EBD065EE573}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
   <si>
     <t>Category</t>
   </si>
@@ -45,27 +45,18 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>(SEO or Accessibility?)</t>
-  </si>
-  <si>
     <t>Accessibility</t>
   </si>
   <si>
     <t>https://www.w3.org/WAI/WCAG21/quickref/?showtechniques=311#language-of-page</t>
   </si>
   <si>
-    <t>The contents of a page title is very important for search engine optimization (SEO)! The page title is used by search engine algorithms to decide the order when listing pages in search results.</t>
-  </si>
-  <si>
     <t>https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links</t>
   </si>
   <si>
     <t>SEO</t>
   </si>
   <si>
-    <t>Always include a title on your website.</t>
-  </si>
-  <si>
     <t>Hidden keywords such as the ones used in the footer of home page are considered a "black hat" technique which might result in the website being banned from search engines results</t>
   </si>
   <si>
@@ -78,50 +69,25 @@
     <t>https://openclassrooms.com/en/courses/6663451-make-your-web-content-accessible/6913058-annotate-mock-ups-and-wireframes-with-accessibility-information</t>
   </si>
   <si>
-    <t>To make the page easier to navigate for assistive technology users, you should define the main regions of your page using either structural HTML elements, ARIA landmark roles, or both.</t>
-  </si>
-  <si>
     <t>Always use appropariate HTML emelent or/and ARIA landmark roles</t>
   </si>
   <si>
     <t>missing structural HTML elements/ARIA landmarks</t>
   </si>
   <si>
-    <t>existing &lt;title&gt; tag in head missing content</t>
-  </si>
-  <si>
     <t>lang attribute in &lt;html&gt; tag set to "default" instead of actual language</t>
   </si>
   <si>
-    <t>WCAG Success Criterion 3.1.1 requires that a page language is specified in a way which may be 'programmatically determined' (i.e. via the lang attribute).</t>
-  </si>
-  <si>
     <t>External links in footer</t>
   </si>
   <si>
-    <t>Avoid placing external links in your footer. If you must link to another website in your footer, use the “nofollow” tag.</t>
-  </si>
-  <si>
     <t>Links to external websites in the footer used to rank up in SEO are considered a "black hat" technique which might result in the website being banned from search engines results</t>
   </si>
   <si>
-    <t>Using text and visuals as one image is preventing assistive technology users to preceive the content as for example readers won't be able to select text. It is also preventing people from modifying fonts and doesn’t respond to changes in color, size, and regular text.</t>
-  </si>
-  <si>
-    <t>Separate the text and place it as HTML content on top of the background or communicate all of the text in the image as alternative text.</t>
-  </si>
-  <si>
     <t>Irrelevant links to partners</t>
   </si>
   <si>
     <t>https://openclassrooms.com/en/courses/3594061-drive-traffic-to-your-website-with-search-engine-optimization-seo/5838332-increase-your-websites-authority</t>
-  </si>
-  <si>
-    <t>A quality link to/from your website should be found among content that is relevant to your profession.
-It should also attract real traffic, meaning that it is on a page real visitors read, not hidden away in some obscure part of the website.</t>
-  </si>
-  <si>
-    <t>Increase your website authority by using only quality links to/from other websites and building relevant partnerships.</t>
   </si>
   <si>
     <t>https://www.w3schools.com/tags/tag_title.asp
@@ -145,18 +111,12 @@
     <t>https://openclassrooms.com/en/courses/3594061-drive-traffic-to-your-website-with-search-engine-optimization-seo/5838156-optimize-the-content-of-your-web-pages</t>
   </si>
   <si>
-    <t>The keywords for the website should be included in titles, &lt;h1&gt; (as an exact match to title) and &lt;h2&gt; tags, paragraphs and alternative text in images where possible.</t>
-  </si>
-  <si>
     <t>Missing keywords in &lt;h1&gt; tag, &lt;h2&gt; tags</t>
   </si>
   <si>
     <t>https://openclassrooms.com/en/courses/1306056-ensure-your-website-meets-technical-seo-requirements/6200762-keep-your-webpages-light</t>
   </si>
   <si>
-    <t>The larger the image, the bigger the file, and the longer it takes for a browser to download. Using not optimized images will slow loading your page for users.</t>
-  </si>
-  <si>
     <t>Always keep your images as light in size as possible</t>
   </si>
   <si>
@@ -166,12 +126,6 @@
     <t>https://www.searchenginejournal.com/on-page-seo/image-optimization/</t>
   </si>
   <si>
-    <t>Image file names alert Google and other search engine crawlers as to the subject matter of the image.</t>
-  </si>
-  <si>
-    <t>Change the file name from the default to help the search engines understand your image and improve your SEO value.</t>
-  </si>
-  <si>
     <t>hidden text/keywords in footer and header</t>
   </si>
   <si>
@@ -179,12 +133,6 @@
   </si>
   <si>
     <t>https://openclassrooms.com/en/courses/6663451-make-your-web-content-accessible/6912083-get-to-know-the-web-content-accessibility-guidelines-wcag</t>
-  </si>
-  <si>
-    <t>Text should be placed as HTML content on top of the background not be hidden behind it.</t>
-  </si>
-  <si>
-    <t>Always make sure that text on your website is not hidden behind other elements and that it is possible to select it.</t>
   </si>
   <si>
     <t>Images size is not optimized and incorrect format</t>
@@ -197,38 +145,156 @@
     <t>CSS and javaScript not minified</t>
   </si>
   <si>
-    <t>Minifying a file means removing unnecessary characters (spaces, line breaks, comments, block separators) from the file, which drastically reduces its file size. It increases the loading speed.</t>
-  </si>
-  <si>
-    <t>Always minify all .css and .js files to increase loading speed.</t>
-  </si>
-  <si>
-    <t>If you don't set the call to your JavaScript files correctly, they will prevent the page from being displayed before it's fully loaded.</t>
-  </si>
-  <si>
     <t>javaScript loading at the same time as HTML</t>
   </si>
   <si>
-    <t>If the execution order is not important and the scripts can be executed as soon as they are available, use the asynchronous method.</t>
-  </si>
-  <si>
     <t>a lot of unsused CSS in the website files</t>
   </si>
   <si>
     <t>https://web.dev/unused-css-rules/?utm_source=lighthouse&amp;utm_medium=devtools</t>
   </si>
   <si>
-    <t>By default, a browser must download, parse, and process all external stylesheets that it encounters before it can display, or render, any content to a user's screen. It wouldn't make sense for a browser to attempt to display content before the stylesheets have been processed, because the stylesheets may contain rules that affect the styling of the page.</t>
-  </si>
-  <si>
     <t>Remove the unused CSS to reduce unnecessary bytes consumed by network activity</t>
+  </si>
+  <si>
+    <t>color contrast of headings and backgroung too low</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/en/courses/6663451-make-your-web-content-accessible/6912752-create-accessible-visual-designs</t>
+  </si>
+  <si>
+    <t>Unused CSS removed</t>
+  </si>
+  <si>
+    <t>Color contrast of headings on main page changed</t>
+  </si>
+  <si>
+    <t>Async function added and scripts moved to end of &lt;body&gt; element</t>
+  </si>
+  <si>
+    <t>All CSS and javaSript files minified</t>
+  </si>
+  <si>
+    <t>Text moved to the front</t>
+  </si>
+  <si>
+    <t>Images names changed to match the content, page2 page name changed to 'contact'</t>
+  </si>
+  <si>
+    <t>Image sizes changed to match their size on website, format changed to .webp</t>
+  </si>
+  <si>
+    <t>Do not use multiple &lt;h1&gt; tags on website</t>
+  </si>
+  <si>
+    <t>&lt;h1&gt; tags changed to correct subheadings (&lt;h2&gt;, &lt;h3&gt; etc.)</t>
+  </si>
+  <si>
+    <t>Include your keyword in multiple elements on the website</t>
+  </si>
+  <si>
+    <t>Irrelevant links removed</t>
+  </si>
+  <si>
+    <t>"nofollow" attribute added to relevant link</t>
+  </si>
+  <si>
+    <t>Images with text replaced with actual text</t>
+  </si>
+  <si>
+    <t>Hidden text removed</t>
+  </si>
+  <si>
+    <t>Empty item removed and actual title added</t>
+  </si>
+  <si>
+    <t>existing &lt;title&gt; tag in head missing content. One of the items in navigation list is empty</t>
+  </si>
+  <si>
+    <t>Language attribute set to "en"</t>
+  </si>
+  <si>
+    <t>WCAG Success Criterion 3.1.1 requires that a page language is specified in a way which may be 'programmatically determined' (i.e. via the lang attribute)</t>
+  </si>
+  <si>
+    <t>The contents of a page title is very important for search engine optimization (SEO)! The page title is used by search engine algorithms to decide the order when listing pages in search results</t>
+  </si>
+  <si>
+    <t>To make the page easier to navigate for assistive technology users, you should define the main regions of your page using either structural HTML elements, ARIA landmark roles, or both</t>
+  </si>
+  <si>
+    <t>&lt;div&gt; elements replaces with structural html elements and ARIA landmark roles added to similar elements to describe their role</t>
+  </si>
+  <si>
+    <t>Using text and visuals as one image is preventing assistive technology users to preceive the content as for example readers won't be able to select text. It is also preventing people from modifying fonts and doesn’t respond to changes in color, size, and regular text</t>
+  </si>
+  <si>
+    <t>Separate the text and place it as HTML content on top of the background or communicate all of the text in the image as alternative text</t>
+  </si>
+  <si>
+    <t>Avoid placing external links in your footer. If you must link to another website in your footer, use the “nofollow” attribute</t>
+  </si>
+  <si>
+    <t>Increase your website authority by using only quality links to/from other websites and building relevant partnerships</t>
+  </si>
+  <si>
+    <t>A quality link to/from your website should be found among content that is relevant to your profession.
+It should also attract real traffic, meaning that it is on a page real visitors read, not hidden away in some obscure part of the website</t>
+  </si>
+  <si>
+    <t>The keywords for the website should be included in titles, &lt;h1&gt; (as an exact match to title) and &lt;h2&gt; tags, paragraphs and alternative text in images where possible</t>
+  </si>
+  <si>
+    <t>There should only be one &lt;h1&gt; tag on website that matches the keyword for the website</t>
+  </si>
+  <si>
+    <t>Keyword changed and included in title, headings, subheadings</t>
+  </si>
+  <si>
+    <t>The larger the image, the bigger the file, and the longer it takes for a browser to download. Using not optimized images will slow loading your page for users</t>
+  </si>
+  <si>
+    <t>Image file names alert Google and other search engine crawlers as to the subject matter of the image</t>
+  </si>
+  <si>
+    <t>Change the file name from the default to help the search engines understand your image and improve your SEO value</t>
+  </si>
+  <si>
+    <t>Text should be placed as HTML content on top of the background not be hidden behind it</t>
+  </si>
+  <si>
+    <t>Always make sure that text on your website is not hidden behind other elements and that it is possible to select it</t>
+  </si>
+  <si>
+    <t>Minifying a file means removing unnecessary characters (spaces, line breaks, comments, block separators) from the file, which drastically reduces its file size. It increases the loading speed</t>
+  </si>
+  <si>
+    <t>Always minify all .css and .js files to increase loading speed</t>
+  </si>
+  <si>
+    <t>If the execution order is not important and the scripts can be executed as soon as they are available, use the asynchronous method</t>
+  </si>
+  <si>
+    <t>If you don't set the call to your JavaScript files correctly, they will prevent the page from being displayed before it's fully loaded</t>
+  </si>
+  <si>
+    <t>By default, a browser must download, parse, and process all external stylesheets that it encounters before it can display, or render, any content to a user's screen. It wouldn't make sense for a browser to attempt to display content before the stylesheets have been processed, because the stylesheets may contain rules that affect the styling of the page</t>
+  </si>
+  <si>
+    <t> The Web Content Accessibility Guidelines (WCAG) require a contrast ratio between text and background of at least 4.5:1 for regular text, and 3:1 for large (18pt) and bold text (14pt) at level AA</t>
+  </si>
+  <si>
+    <t>Check the colors contrast for the pallette you use</t>
+  </si>
+  <si>
+    <t>Always include a title on your website. Never leave empty html elements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -269,14 +335,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -294,40 +352,30 @@
       <scheme val="major"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="major"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1" tint="0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="major"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,23 +400,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -391,74 +438,240 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="4" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Explanatory Text" xfId="5" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="4" builtinId="21"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
+    <cellStyle name="Output" xfId="3" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -674,7 +887,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -682,355 +895,388 @@
     <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="40.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="44.33203125" style="1" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" style="1" customWidth="1"/>
     <col min="27" max="16384" width="11.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="E4" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13" t="b">
-        <v>0</v>
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>72</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="14" t="b">
-        <v>0</v>
+      <c r="A12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="14" t="b">
-        <v>0</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="63" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>40</v>
+      <c r="B17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1999,7 +2245,15 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{1DC8CB37-69B6-4565-9010-DCE4B8A15795}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{AF8A41B2-3E5F-4EEE-9503-D6E0A765755A}"/>
+    <hyperlink ref="F10" r:id="rId3" xr:uid="{35B6B459-00B1-4D12-B144-40349AC1E691}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{2B9EDEC1-38AF-47A7-A8D7-89ED3374622D}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{51AFEB1E-BE4C-4866-B249-3A68E430DEF2}"/>
+    <hyperlink ref="F2" r:id="rId6" location="language-of-page" xr:uid="{D30246E3-63C7-41A6-BD90-DB643A4E784A}"/>
+  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>